<commit_message>
fixed bugs and locked cells
</commit_message>
<xml_diff>
--- a/full_predictions.xlsx
+++ b/full_predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jl2964/my_tests/worldcup_predictions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174B35A4-2851-0C49-B01E-F13D4E65400A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E7F550-655E-B448-B560-35D4D608DC30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4172" uniqueCount="92">
   <si>
     <t>Team</t>
   </si>
@@ -263,15 +263,48 @@
   <si>
     <t>Runner-up of B</t>
   </si>
+  <si>
+    <t>Runner-up of C</t>
+  </si>
+  <si>
+    <t>Winner of D</t>
+  </si>
+  <si>
+    <t>Winner of E</t>
+  </si>
+  <si>
+    <t>Runner-up of F</t>
+  </si>
+  <si>
+    <t>Runner-up of G</t>
+  </si>
+  <si>
+    <t>Winner of H</t>
+  </si>
+  <si>
+    <t>Winner of C</t>
+  </si>
+  <si>
+    <t>Runner-up of D</t>
+  </si>
+  <si>
+    <t>Runner-up of H</t>
+  </si>
+  <si>
+    <t>Winner of G</t>
+  </si>
+  <si>
+    <t>Winner of F</t>
+  </si>
+  <si>
+    <t>Runner-up of E</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,13 +327,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -312,17 +357,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1466,458 +1514,2206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03A69B2-2FA3-7E43-9559-C7DC7B1D5793}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A56" sqref="A56:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.21679999999999999</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>D2-B2</f>
         <v>0.28260000000000002</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.49940000000000001</v>
       </c>
-      <c r="E2" s="3">
-        <f>B2*($C$8*VLOOKUP($A$8, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + $C$9*VLOOKUP($A$9, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + $C$10*VLOOKUP($A$10, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + $C$11*VLOOKUP($A$11, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+      <c r="E2" s="2">
+        <f>B2*(C8*VLOOKUP(A8, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C9*VLOOKUP(A9, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C10*VLOOKUP(A10, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C11*VLOOKUP(A11, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
         <v>7.0158613114117196E-2</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.1036</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C10" si="0">D3-B3</f>
         <v>0.18679999999999999</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.29039999999999999</v>
       </c>
-      <c r="E3" s="3">
-        <f>B3*($C$8*VLOOKUP($A$8, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + $C$9*VLOOKUP($A$9, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + $C$10*VLOOKUP($A$10, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + $C$11*VLOOKUP($A$11, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+      <c r="E3" s="2">
+        <f>B3*(C8*VLOOKUP(A8, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C9*VLOOKUP(A9, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C10*VLOOKUP(A10, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C11*VLOOKUP(A11, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
         <v>2.1560551582548132E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.18179999999999999</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>0.26580000000000004</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.4476</v>
       </c>
-      <c r="E4" s="3">
-        <f>B4*($C$8*VLOOKUP($A$8, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + $C$9*VLOOKUP($A$9, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + $C$10*VLOOKUP($A$10, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + $C$11*VLOOKUP($A$11, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+      <c r="E4" s="2">
+        <f>B4*(C8*VLOOKUP(A8, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C9*VLOOKUP(A9, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C10*VLOOKUP(A10, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C11*VLOOKUP(A11, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
         <v>5.7137825352393028E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.49780000000000002</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>0.26479999999999992</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.76259999999999994</v>
       </c>
-      <c r="E5" s="3">
-        <f>B5*($C$8*VLOOKUP($A$8, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + $C$9*VLOOKUP($A$9, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + $C$10*VLOOKUP($A$10, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + $C$11*VLOOKUP($A$11, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+      <c r="E5" s="2">
+        <f>B5*(C8*VLOOKUP(A8, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C9*VLOOKUP(A9, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C10*VLOOKUP(A10, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C11*VLOOKUP(A11, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
         <v>0.23457191582764303</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2">
         <f t="shared" ref="B6:D6" si="1">SUM(B2:B5)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f>SUM(E2:E5)</f>
         <v>0.38342890587670142</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0.24510000000000001</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>D8-B8</f>
         <v>0.27490000000000003</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.52</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f>C8*(B2*VLOOKUP(A2, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B3*VLOOKUP(A3, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B4*VLOOKUP(A4, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B5*VLOOKUP(A5, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
         <v>0.17171746948532104</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.44869999999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f>D9-B9</f>
         <v>0.26890000000000003</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.71760000000000002</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f>C9*(B2*VLOOKUP(A2, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B3*VLOOKUP(A3, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B4*VLOOKUP(A4, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B5*VLOOKUP(A5, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
         <v>0.19710482450933728</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.19</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f>D10-B10</f>
         <v>0.2555</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.44550000000000001</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f>C10*(B2*VLOOKUP(A2, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B3*VLOOKUP(A3, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B4*VLOOKUP(A4, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B5*VLOOKUP(A5, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
         <v>0.14944151217706397</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0.1162</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f>D11-B11</f>
         <v>0.20070000000000002</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.31690000000000002</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f>C11*(B2*VLOOKUP(A2, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B3*VLOOKUP(A3, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B4*VLOOKUP(A4, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B5*VLOOKUP(A5, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
         <v>9.830728795157638E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="3">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2">
         <f t="shared" ref="B12" si="2">SUM(B8:B11)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f t="shared" ref="C12" si="3">SUM(C8:C11)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f t="shared" ref="D12" si="4">SUM(D8:D11)</f>
         <v>2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f>SUM(E8:E11)</f>
         <v>0.61657109412329869</v>
       </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
         <f>E12+E6</f>
         <v>1</v>
       </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>0.21679999999999999</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f>D15-B15</f>
         <v>0.28260000000000002</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>0.49940000000000001</v>
       </c>
-      <c r="E15" s="3">
-        <f>C15*($B$21*VLOOKUP($A$21, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + $B$22*VLOOKUP($A$22, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + $B$23*VLOOKUP($A$23, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + $B$24*VLOOKUP($A$24, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+      <c r="E15" s="2">
+        <f>C15*(B21*VLOOKUP(A21, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B22*VLOOKUP(A22, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B23*VLOOKUP(A23, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B24*VLOOKUP(A24, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
         <v>8.2284952200555594E-2</v>
       </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>0.1036</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f t="shared" ref="C16:C18" si="5">D16-B16</f>
         <v>0.18679999999999999</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>0.29039999999999999</v>
       </c>
-      <c r="E16" s="3">
-        <f>C16*($B$21*VLOOKUP($A$21, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + $B$22*VLOOKUP($A$22, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + $B$23*VLOOKUP($A$23, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + $B$24*VLOOKUP($A$24, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+      <c r="E16" s="2">
+        <f>C16*(B21*VLOOKUP(A21, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B22*VLOOKUP(A22, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B23*VLOOKUP(A23, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B24*VLOOKUP(A24, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
         <v>3.3837264602812923E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>0.18179999999999999</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <f t="shared" si="5"/>
         <v>0.26580000000000004</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>0.4476</v>
       </c>
-      <c r="E17" s="3">
-        <f>C17*($B$21*VLOOKUP($A$21, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + $B$22*VLOOKUP($A$22, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + $B$23*VLOOKUP($A$23, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + $B$24*VLOOKUP($A$24, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+      <c r="E17" s="2">
+        <f>C17*(B21*VLOOKUP(A21, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B22*VLOOKUP(A22, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B23*VLOOKUP(A23, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B24*VLOOKUP(A24, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
         <v>7.5444129042134156E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.49780000000000002</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <f t="shared" si="5"/>
         <v>0.26479999999999992</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>0.76259999999999994</v>
       </c>
-      <c r="E18" s="3">
-        <f>C18*($B$21*VLOOKUP($A$21, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + $B$22*VLOOKUP($A$22, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + $B$23*VLOOKUP($A$23, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + $B$24*VLOOKUP($A$24, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+      <c r="E18" s="2">
+        <f>C18*(B21*VLOOKUP(A21, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B22*VLOOKUP(A22, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B23*VLOOKUP(A23, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B24*VLOOKUP(A24, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
         <v>0.11514190333256598</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="3">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2">
         <f t="shared" ref="B19" si="6">SUM(B15:B18)</f>
         <v>1</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <f t="shared" ref="C19" si="7">SUM(C15:C18)</f>
         <v>1</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <f t="shared" ref="D19" si="8">SUM(D15:D18)</f>
         <v>2</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f>SUM(E15:E18)</f>
         <v>0.30670824917806866</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>0.24510000000000001</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <f>D21-B21</f>
         <v>0.27490000000000003</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>0.52</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f>B21*(C15*VLOOKUP(A15, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C16*VLOOKUP(A16, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C17*VLOOKUP(A17, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C18*VLOOKUP(A18, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
         <v>0.16468071187978453</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>0.44869999999999999</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <f>D22-B22</f>
         <v>0.26890000000000003</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>0.71760000000000002</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f>B22*(C15*VLOOKUP(A15, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C16*VLOOKUP(A16, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C17*VLOOKUP(A17, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C18*VLOOKUP(A18, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
         <v>0.34628468159497033</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>0.19</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <f>D23-B23</f>
         <v>0.2555</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>0.44550000000000001</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f>B23*(C15*VLOOKUP(A15, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C16*VLOOKUP(A16, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C17*VLOOKUP(A17, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C18*VLOOKUP(A18, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
         <v>0.11971051370413367</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>0.1162</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <f>D24-B24</f>
         <v>0.20070000000000002</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>0.31690000000000002</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f>B24*(C15*VLOOKUP(A15, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C16*VLOOKUP(A16, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C17*VLOOKUP(A17, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C18*VLOOKUP(A18, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
         <v>6.2615843643042735E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="3">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2">
         <f t="shared" ref="B25" si="9">SUM(B21:B24)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <f t="shared" ref="C25" si="10">SUM(C21:C24)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <f t="shared" ref="D25" si="11">SUM(D21:D24)</f>
         <v>2</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f>SUM(E21:E24)</f>
         <v>0.69329175082193129</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E26" s="3">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2">
         <f>E25+E19</f>
         <v>1</v>
       </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C29" s="2">
+        <f>D29-B29</f>
+        <v>0.28260000000000002</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E29" s="2">
+        <f>B29*(C35*VLOOKUP(A35, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C36*VLOOKUP(A36, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C37*VLOOKUP(A37, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C38*VLOOKUP(A38, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+        <v>7.0158613114117196E-2</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.1036</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" ref="C30:C32" si="12">D30-B30</f>
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.29039999999999999</v>
+      </c>
+      <c r="E30" s="2">
+        <f>B30*(C35*VLOOKUP(A35, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C36*VLOOKUP(A36, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C37*VLOOKUP(A37, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C38*VLOOKUP(A38, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+        <v>2.1560551582548132E-2</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="12"/>
+        <v>0.26580000000000004</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.4476</v>
+      </c>
+      <c r="E31" s="2">
+        <f>B31*(C35*VLOOKUP(A35, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C36*VLOOKUP(A36, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C37*VLOOKUP(A37, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C38*VLOOKUP(A38, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+        <v>5.7137825352393028E-2</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.49780000000000002</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="12"/>
+        <v>0.26479999999999992</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="E32" s="2">
+        <f>B32*(C35*VLOOKUP(A35, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C36*VLOOKUP(A36, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C37*VLOOKUP(A37, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C38*VLOOKUP(A38, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+        <v>0.23457191582764303</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2">
+        <f t="shared" ref="B33" si="13">SUM(B29:B32)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" ref="C33" si="14">SUM(C29:C32)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" ref="D33" si="15">SUM(D29:D32)</f>
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <f>SUM(E29:E32)</f>
+        <v>0.38342890587670142</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="C35" s="2">
+        <f>D35-B35</f>
+        <v>0.27490000000000003</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E35" s="2">
+        <f>C35*(B29*VLOOKUP(A29, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B30*VLOOKUP(A30, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B31*VLOOKUP(A31, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B32*VLOOKUP(A32, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
+        <v>0.17171746948532104</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C36" s="2">
+        <f>D36-B36</f>
+        <v>0.26890000000000003</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="E36" s="2">
+        <f>C36*(B29*VLOOKUP(A29, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B30*VLOOKUP(A30, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B31*VLOOKUP(A31, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B32*VLOOKUP(A32, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
+        <v>0.19710482450933728</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C37" s="2">
+        <f>D37-B37</f>
+        <v>0.2555</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="E37" s="2">
+        <f>C37*(B29*VLOOKUP(A29, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B30*VLOOKUP(A30, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B31*VLOOKUP(A31, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B32*VLOOKUP(A32, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
+        <v>0.14944151217706397</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.1162</v>
+      </c>
+      <c r="C38" s="2">
+        <f>D38-B38</f>
+        <v>0.20070000000000002</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E38" s="2">
+        <f>C38*(B29*VLOOKUP(A29, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B30*VLOOKUP(A30, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B31*VLOOKUP(A31, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B32*VLOOKUP(A32, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>9.830728795157638E-2</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2">
+        <f t="shared" ref="B39" si="16">SUM(B35:B38)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" ref="C39" si="17">SUM(C35:C38)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="18">SUM(D35:D38)</f>
+        <v>2</v>
+      </c>
+      <c r="E39" s="2">
+        <f>SUM(E35:E38)</f>
+        <v>0.61657109412329869</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2">
+        <f>E39+E33</f>
+        <v>1</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C42" s="2">
+        <f>D42-B42</f>
+        <v>0.28260000000000002</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E42" s="2">
+        <f>C42*(B48*VLOOKUP(A48, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B49*VLOOKUP(A49, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B50*VLOOKUP(A50, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B51*VLOOKUP(A51, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+        <v>8.2284952200555594E-2</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.1036</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" ref="C43:C45" si="19">D43-B43</f>
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.29039999999999999</v>
+      </c>
+      <c r="E43" s="2">
+        <f>C43*(B48*VLOOKUP(A48, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B49*VLOOKUP(A49, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B50*VLOOKUP(A50, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B51*VLOOKUP(A51, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+        <v>3.3837264602812923E-2</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="19"/>
+        <v>0.26580000000000004</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.4476</v>
+      </c>
+      <c r="E44" s="2">
+        <f>C44*(B48*VLOOKUP(A48, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B49*VLOOKUP(A49, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B50*VLOOKUP(A50, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B51*VLOOKUP(A51, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+        <v>7.5444129042134156E-2</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.49780000000000002</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="19"/>
+        <v>0.26479999999999992</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="E45" s="2">
+        <f>C45*(B48*VLOOKUP(A48, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B49*VLOOKUP(A49, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B50*VLOOKUP(A50, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B51*VLOOKUP(A51, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+        <v>0.11514190333256598</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2">
+        <f t="shared" ref="B46" si="20">SUM(B42:B45)</f>
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" ref="C46" si="21">SUM(C42:C45)</f>
+        <v>1</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" ref="D46" si="22">SUM(D42:D45)</f>
+        <v>2</v>
+      </c>
+      <c r="E46" s="2">
+        <f>SUM(E42:E45)</f>
+        <v>0.30670824917806866</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="C48" s="2">
+        <f>D48-B48</f>
+        <v>0.27490000000000003</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E48" s="2">
+        <f>B48*(C42*VLOOKUP(A42, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C43*VLOOKUP(A43, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C44*VLOOKUP(A44, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C45*VLOOKUP(A45, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
+        <v>0.16468071187978453</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C49" s="2">
+        <f>D49-B49</f>
+        <v>0.26890000000000003</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="E49" s="2">
+        <f>B49*(C42*VLOOKUP(A42, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C43*VLOOKUP(A43, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C44*VLOOKUP(A44, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C45*VLOOKUP(A45, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
+        <v>0.34628468159497033</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C50" s="2">
+        <f>D50-B50</f>
+        <v>0.2555</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="E50" s="2">
+        <f>B50*(C42*VLOOKUP(A42, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C43*VLOOKUP(A43, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C44*VLOOKUP(A44, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C45*VLOOKUP(A45, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
+        <v>0.11971051370413367</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.1162</v>
+      </c>
+      <c r="C51" s="2">
+        <f>D51-B51</f>
+        <v>0.20070000000000002</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E51" s="2">
+        <f>B51*(C42*VLOOKUP(A42, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C43*VLOOKUP(A43, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C44*VLOOKUP(A44, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C45*VLOOKUP(A45, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>6.2615843643042735E-2</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2">
+        <f t="shared" ref="B52" si="23">SUM(B48:B51)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" ref="C52" si="24">SUM(C48:C51)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" ref="D52" si="25">SUM(D48:D51)</f>
+        <v>2</v>
+      </c>
+      <c r="E52" s="2">
+        <f>SUM(E48:E51)</f>
+        <v>0.69329175082193129</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2">
+        <f>E52+E46</f>
+        <v>1</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="C56" s="2">
+        <f>D56-B56</f>
+        <v>0.27490000000000003</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E56" s="2">
+        <f>B56*(C62*VLOOKUP(A62, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C63*VLOOKUP(A63, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C64*VLOOKUP(A64, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C65*VLOOKUP(A65, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
+        <v>0.16468071187978453</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C57" s="2">
+        <f>D57-B57</f>
+        <v>0.26890000000000003</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="E57" s="2">
+        <f>B57*(C62*VLOOKUP(A62, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C63*VLOOKUP(A63, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C64*VLOOKUP(A64, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C65*VLOOKUP(A65, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
+        <v>0.34628468159497033</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C58" s="2">
+        <f>D58-B58</f>
+        <v>0.2555</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="E58" s="2">
+        <f>B58*(C62*VLOOKUP(A62, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C63*VLOOKUP(A63, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C64*VLOOKUP(A64, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C65*VLOOKUP(A65, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
+        <v>0.11971051370413367</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.1162</v>
+      </c>
+      <c r="C59" s="2">
+        <f>D59-B59</f>
+        <v>0.20070000000000002</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E59" s="2">
+        <f>B59*(C62*VLOOKUP(A62, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C63*VLOOKUP(A63, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C64*VLOOKUP(A64, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C65*VLOOKUP(A65, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>6.2615843643042735E-2</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="2">
+        <f t="shared" ref="B60" si="26">SUM(B56:B59)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" ref="C60" si="27">SUM(C56:C59)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" ref="D60" si="28">SUM(D56:D59)</f>
+        <v>2</v>
+      </c>
+      <c r="E60" s="2">
+        <f>SUM(E56:E59)</f>
+        <v>0.69329175082193129</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C62" s="2">
+        <f>D62-B62</f>
+        <v>0.28260000000000002</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E62" s="2">
+        <f>C62*(B56*VLOOKUP(A56, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B57*VLOOKUP(A57, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B58*VLOOKUP(A58, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B59*VLOOKUP(A59, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+        <v>8.2284952200555594E-2</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0.1036</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" ref="C63:C65" si="29">D63-B63</f>
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.29039999999999999</v>
+      </c>
+      <c r="E63" s="2">
+        <f>C63*(B56*VLOOKUP(A56, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B57*VLOOKUP(A57, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B58*VLOOKUP(A58, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B59*VLOOKUP(A59, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+        <v>3.3837264602812923E-2</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="29"/>
+        <v>0.26580000000000004</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.4476</v>
+      </c>
+      <c r="E64" s="2">
+        <f>C64*(B56*VLOOKUP(A56, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B57*VLOOKUP(A57, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B58*VLOOKUP(A58, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B59*VLOOKUP(A59, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+        <v>7.5444129042134156E-2</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.49780000000000002</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="29"/>
+        <v>0.26479999999999992</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="E65" s="2">
+        <f>C65*(B56*VLOOKUP(A56, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B57*VLOOKUP(A57, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B58*VLOOKUP(A58, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B59*VLOOKUP(A59, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+        <v>0.11514190333256598</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2">
+        <f t="shared" ref="B66" si="30">SUM(B62:B65)</f>
+        <v>1</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" ref="C66" si="31">SUM(C62:C65)</f>
+        <v>1</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" ref="D66" si="32">SUM(D62:D65)</f>
+        <v>2</v>
+      </c>
+      <c r="E66" s="2">
+        <f>SUM(E62:E65)</f>
+        <v>0.30670824917806866</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E67" s="2">
+        <f>E60+E66</f>
+        <v>1</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="J68" s="4"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C69" s="2">
+        <f>D69-B69</f>
+        <v>0.28260000000000002</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E69" s="2">
+        <f>C69*(B75*VLOOKUP(A75, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B76*VLOOKUP(A76, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B77*VLOOKUP(A77, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B78*VLOOKUP(A78, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+        <v>8.2284952200555594E-2</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.1036</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" ref="C70:C72" si="33">D70-B70</f>
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.29039999999999999</v>
+      </c>
+      <c r="E70" s="2">
+        <f>C70*(B75*VLOOKUP(A75, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B76*VLOOKUP(A76, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B77*VLOOKUP(A77, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B78*VLOOKUP(A78, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+        <v>3.3837264602812923E-2</v>
+      </c>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="33"/>
+        <v>0.26580000000000004</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.4476</v>
+      </c>
+      <c r="E71" s="2">
+        <f>C71*(B75*VLOOKUP(A75, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B76*VLOOKUP(A76, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B77*VLOOKUP(A77, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B78*VLOOKUP(A78, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+        <v>7.5444129042134156E-2</v>
+      </c>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.49780000000000002</v>
+      </c>
+      <c r="C72" s="2">
+        <f t="shared" si="33"/>
+        <v>0.26479999999999992</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="E72" s="2">
+        <f>C72*(B75*VLOOKUP(A75, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B76*VLOOKUP(A76, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B77*VLOOKUP(A77, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B78*VLOOKUP(A78, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+        <v>0.11514190333256598</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2">
+        <f t="shared" ref="B73" si="34">SUM(B69:B72)</f>
+        <v>1</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" ref="C73" si="35">SUM(C69:C72)</f>
+        <v>1</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" ref="D73" si="36">SUM(D69:D72)</f>
+        <v>2</v>
+      </c>
+      <c r="E73" s="2">
+        <f>SUM(E69:E72)</f>
+        <v>0.30670824917806866</v>
+      </c>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="C75" s="2">
+        <f>D75-B75</f>
+        <v>0.27490000000000003</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E75" s="2">
+        <f>B75*(C69*VLOOKUP(A69, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C70*VLOOKUP(A70, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C71*VLOOKUP(A71, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C72*VLOOKUP(A72, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
+        <v>0.16468071187978453</v>
+      </c>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C76" s="2">
+        <f>D76-B76</f>
+        <v>0.26890000000000003</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="E76" s="2">
+        <f>B76*(C69*VLOOKUP(A69, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C70*VLOOKUP(A70, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C71*VLOOKUP(A71, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C72*VLOOKUP(A72, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
+        <v>0.34628468159497033</v>
+      </c>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C77" s="2">
+        <f>D77-B77</f>
+        <v>0.2555</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="E77" s="2">
+        <f>B77*(C69*VLOOKUP(A69, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C70*VLOOKUP(A70, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C71*VLOOKUP(A71, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C72*VLOOKUP(A72, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
+        <v>0.11971051370413367</v>
+      </c>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.1162</v>
+      </c>
+      <c r="C78" s="2">
+        <f>D78-B78</f>
+        <v>0.20070000000000002</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E78" s="2">
+        <f>B78*(C69*VLOOKUP(A69, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C70*VLOOKUP(A70, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C71*VLOOKUP(A71, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C72*VLOOKUP(A72, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>6.2615843643042735E-2</v>
+      </c>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2">
+        <f t="shared" ref="B79" si="37">SUM(B75:B78)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C79" s="2">
+        <f t="shared" ref="C79" si="38">SUM(C75:C78)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" ref="D79" si="39">SUM(D75:D78)</f>
+        <v>2</v>
+      </c>
+      <c r="E79" s="2">
+        <f>SUM(E75:E78)</f>
+        <v>0.69329175082193129</v>
+      </c>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2">
+        <f>E79+E73</f>
+        <v>1</v>
+      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C83" s="2">
+        <f>D83-B83</f>
+        <v>0.28260000000000002</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E83" s="2">
+        <f>B83*(C89*VLOOKUP(A89, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C90*VLOOKUP(A90, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C91*VLOOKUP(A91, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C92*VLOOKUP(A92, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+        <v>7.0158613114117196E-2</v>
+      </c>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.1036</v>
+      </c>
+      <c r="C84" s="2">
+        <f t="shared" ref="C84:C86" si="40">D84-B84</f>
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.29039999999999999</v>
+      </c>
+      <c r="E84" s="2">
+        <f>B84*(C89*VLOOKUP(A89, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C90*VLOOKUP(A90, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C91*VLOOKUP(A91, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C92*VLOOKUP(A92, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+        <v>2.1560551582548132E-2</v>
+      </c>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="C85" s="2">
+        <f t="shared" si="40"/>
+        <v>0.26580000000000004</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.4476</v>
+      </c>
+      <c r="E85" s="2">
+        <f>B85*(C89*VLOOKUP(A89, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C90*VLOOKUP(A90, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C91*VLOOKUP(A91, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C92*VLOOKUP(A92, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+        <v>5.7137825352393028E-2</v>
+      </c>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.49780000000000002</v>
+      </c>
+      <c r="C86" s="2">
+        <f t="shared" si="40"/>
+        <v>0.26479999999999992</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="E86" s="2">
+        <f>B86*(C89*VLOOKUP(A89, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C90*VLOOKUP(A90, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C91*VLOOKUP(A91, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C92*VLOOKUP(A92, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+        <v>0.23457191582764303</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2">
+        <f t="shared" ref="B87" si="41">SUM(B83:B86)</f>
+        <v>1</v>
+      </c>
+      <c r="C87" s="2">
+        <f t="shared" ref="C87" si="42">SUM(C83:C86)</f>
+        <v>1</v>
+      </c>
+      <c r="D87" s="2">
+        <f t="shared" ref="D87" si="43">SUM(D83:D86)</f>
+        <v>2</v>
+      </c>
+      <c r="E87" s="2">
+        <f>SUM(E83:E86)</f>
+        <v>0.38342890587670142</v>
+      </c>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="C89" s="2">
+        <f>D89-B89</f>
+        <v>0.27490000000000003</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E89" s="2">
+        <f>C89*(B83*VLOOKUP(A83, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B84*VLOOKUP(A84, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B85*VLOOKUP(A85, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + B86*VLOOKUP(A86, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
+        <v>0.17171746948532104</v>
+      </c>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C90" s="2">
+        <f>D90-B90</f>
+        <v>0.26890000000000003</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="E90" s="2">
+        <f>C90*(B83*VLOOKUP(A83, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B84*VLOOKUP(A84, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B85*VLOOKUP(A85, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + B86*VLOOKUP(A86, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
+        <v>0.19710482450933728</v>
+      </c>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C91" s="2">
+        <f>D91-B91</f>
+        <v>0.2555</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="E91" s="2">
+        <f>C91*(B83*VLOOKUP(A83, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B84*VLOOKUP(A84, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B85*VLOOKUP(A85, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + B86*VLOOKUP(A86, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
+        <v>0.14944151217706397</v>
+      </c>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.1162</v>
+      </c>
+      <c r="C92" s="2">
+        <f>D92-B92</f>
+        <v>0.20070000000000002</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E92" s="2">
+        <f>C92*(B83*VLOOKUP(A83, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B84*VLOOKUP(A84, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B85*VLOOKUP(A85, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + B86*VLOOKUP(A86, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>9.830728795157638E-2</v>
+      </c>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2">
+        <f t="shared" ref="B93" si="44">SUM(B89:B92)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" ref="C93" si="45">SUM(C89:C92)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" ref="D93" si="46">SUM(D89:D92)</f>
+        <v>2</v>
+      </c>
+      <c r="E93" s="2">
+        <f>SUM(E89:E92)</f>
+        <v>0.61657109412329869</v>
+      </c>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2">
+        <f>E93+E87</f>
+        <v>1</v>
+      </c>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="C96" s="2">
+        <f>D96-B96</f>
+        <v>0.28260000000000002</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="E96" s="2">
+        <f>C96*(B102*VLOOKUP(A102, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B103*VLOOKUP(A103, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B104*VLOOKUP(A104, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + B105*VLOOKUP(A105, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
+        <v>8.2284952200555594E-2</v>
+      </c>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.1036</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" ref="C97:C99" si="47">D97-B97</f>
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.29039999999999999</v>
+      </c>
+      <c r="E97" s="2">
+        <f>C97*(B102*VLOOKUP(A102, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B103*VLOOKUP(A103, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B104*VLOOKUP(A104, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + B105*VLOOKUP(A105, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
+        <v>3.3837264602812923E-2</v>
+      </c>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="47"/>
+        <v>0.26580000000000004</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.4476</v>
+      </c>
+      <c r="E98" s="2">
+        <f>C98*(B102*VLOOKUP(A102, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B103*VLOOKUP(A103, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B104*VLOOKUP(A104, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + B105*VLOOKUP(A105, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
+        <v>7.5444129042134156E-2</v>
+      </c>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.49780000000000002</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="47"/>
+        <v>0.26479999999999992</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="E99" s="2">
+        <f>C99*(B102*VLOOKUP(A102, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B103*VLOOKUP(A103, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B104*VLOOKUP(A104, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + B105*VLOOKUP(A105, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
+        <v>0.11514190333256598</v>
+      </c>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2">
+        <f t="shared" ref="B100" si="48">SUM(B96:B99)</f>
+        <v>1</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" ref="C100" si="49">SUM(C96:C99)</f>
+        <v>1</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" ref="D100" si="50">SUM(D96:D99)</f>
+        <v>2</v>
+      </c>
+      <c r="E100" s="2">
+        <f>SUM(E96:E99)</f>
+        <v>0.30670824917806866</v>
+      </c>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="C102" s="2">
+        <f>D102-B102</f>
+        <v>0.27490000000000003</v>
+      </c>
+      <c r="D102" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E102" s="2">
+        <f>B102*(C96*VLOOKUP(A96, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C97*VLOOKUP(A97, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C98*VLOOKUP(A98, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C99*VLOOKUP(A99, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
+        <v>0.16468071187978453</v>
+      </c>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="C103" s="2">
+        <f>D103-B103</f>
+        <v>0.26890000000000003</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="E103" s="2">
+        <f>B103*(C96*VLOOKUP(A96, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C97*VLOOKUP(A97, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C98*VLOOKUP(A98, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C99*VLOOKUP(A99, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
+        <v>0.34628468159497033</v>
+      </c>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="C104" s="2">
+        <f>D104-B104</f>
+        <v>0.2555</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="E104" s="2">
+        <f>B104*(C96*VLOOKUP(A96, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C97*VLOOKUP(A97, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C98*VLOOKUP(A98, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C99*VLOOKUP(A99, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
+        <v>0.11971051370413367</v>
+      </c>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.1162</v>
+      </c>
+      <c r="C105" s="2">
+        <f>D105-B105</f>
+        <v>0.20070000000000002</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E105" s="2">
+        <f>B105*(C96*VLOOKUP(A96, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C97*VLOOKUP(A97, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C98*VLOOKUP(A98, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C99*VLOOKUP(A99, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>6.2615843643042735E-2</v>
+      </c>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2">
+        <f t="shared" ref="B106" si="51">SUM(B102:B105)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C106" s="2">
+        <f t="shared" ref="C106" si="52">SUM(C102:C105)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" ref="D106" si="53">SUM(D102:D105)</f>
+        <v>2</v>
+      </c>
+      <c r="E106" s="2">
+        <f>SUM(E102:E105)</f>
+        <v>0.69329175082193129</v>
+      </c>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2">
+        <f>E106+E100</f>
+        <v>1</v>
+      </c>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E110" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
one round of qf done
</commit_message>
<xml_diff>
--- a/full_predictions.xlsx
+++ b/full_predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Liu\Documents\SW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5144342C-40C5-403D-8E8F-80464A1BEB0A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AC9C92-CDC9-47FD-BBFC-B96CA6E5C94E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="38400" windowHeight="19656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,25 +423,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -453,22 +441,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -808,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:G17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" activeCellId="1" sqref="A18:G21 A26:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80072,45 +80054,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03A69B2-2FA3-7E43-9559-C7DC7B1D5793}">
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:A99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="9" width="11.5546875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2">
@@ -80127,15 +80112,16 @@
         <f>C2*(D8*VLOOKUP(B8, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + D9*VLOOKUP(B9, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + D10*VLOOKUP(B10, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + D11*VLOOKUP(B11, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
         <v>7.0158613114117196E-2</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G2" s="2">
+        <f>F2*(F15*VLOOKUP(B15,'Match Predictions'!$D$2:$Y$32,21,FALSE)+F16*VLOOKUP(B16,'Match Predictions'!$D$2:$Y$32,21,FALSE)+F17*VLOOKUP(B17,'Match Predictions'!$D$2:$Y$32,21,FALSE)+F18*VLOOKUP(B18,'Match Predictions'!$D$2:$Y$32,21,FALSE)+(F21*VLOOKUP(B21,'Match Predictions'!$D$2:$Y$32,21,FALSE)+F22*VLOOKUP(B22,'Match Predictions'!$D$2:$Y$32,21,FALSE)+F23*VLOOKUP(B23,'Match Predictions'!$D$2:$Y$32,21,FALSE)+F24*VLOOKUP(B24,'Match Predictions'!$D$2:$Y$32,21,FALSE)))</f>
+        <v>2.0542837139830517E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2">
@@ -80152,15 +80138,16 @@
         <f>C3*(D8*VLOOKUP(B8, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + D9*VLOOKUP(B9, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + D10*VLOOKUP(B10, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + D11*VLOOKUP(B11, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
         <v>2.1560551582548132E-2</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <f>F3*(F15*VLOOKUP(B15, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + F16*VLOOKUP(B16, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + F17*VLOOKUP(B17, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + F18*VLOOKUP(B18, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) +(F21*VLOOKUP(B21, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + F22*VLOOKUP(B22, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + F23*VLOOKUP(B23, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + F24*VLOOKUP(B24, 'Match Predictions'!$D$33:$Y$63, 21, FALSE)))</f>
+        <v>4.0005200786548982E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
@@ -80177,15 +80164,16 @@
         <f>C4*(D8*VLOOKUP(B8, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + D9*VLOOKUP(B9, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + D10*VLOOKUP(B10, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + D11*VLOOKUP(B11, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
         <v>5.7137825352393028E-2</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <f>F4*(F15*VLOOKUP(B15, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + F16*VLOOKUP(B16, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + F17*VLOOKUP(B17, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + F18*VLOOKUP(B18, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) +(F21*VLOOKUP(B21, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + F22*VLOOKUP(B22, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + F23*VLOOKUP(B23, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + F24*VLOOKUP(B24, 'Match Predictions'!$D$64:$Y$94, 21, FALSE)))</f>
+        <v>1.629454929442525E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2">
@@ -80202,12 +80190,12 @@
         <f>C5*(D8*VLOOKUP(B8, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + D9*VLOOKUP(B9, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + D10*VLOOKUP(B10, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + D11*VLOOKUP(B11, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
         <v>0.23457191582764303</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
+      <c r="G5" s="2">
+        <f>F5*(F15*VLOOKUP(B15, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + F16*VLOOKUP(B16, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + F17*VLOOKUP(B17, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + F18*VLOOKUP(B18, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) +(F21*VLOOKUP(B21, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + F22*VLOOKUP(B22, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + F23*VLOOKUP(B23, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + F24*VLOOKUP(B24, 'Match Predictions'!$D$95:$Y$125, 21, FALSE)))</f>
+        <v>0.10097166678300752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <f t="shared" ref="C6:E6" si="1">SUM(C2:C5)</f>
         <v>1</v>
@@ -80224,25 +80212,21 @@
         <f>SUM(F2:F5)</f>
         <v>0.38342890587670142</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>79</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2">
@@ -80259,14 +80243,16 @@
         <f>D8*(C2*VLOOKUP(B2, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C3*VLOOKUP(B3, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C4*VLOOKUP(B4, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C5*VLOOKUP(B5, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
         <v>0.17171746948532104</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <f>F8*(F15*VLOOKUP(B15, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + F16*VLOOKUP(B16, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + F17*VLOOKUP(B17, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + F18*VLOOKUP(B18, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) +(F21*VLOOKUP(B21, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + F22*VLOOKUP(B22, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + F23*VLOOKUP(B23, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + F24*VLOOKUP(B24, 'Match Predictions'!$D$126:$Y$156, 21, FALSE)))</f>
+        <v>7.8883488334765356E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2">
@@ -80283,14 +80269,16 @@
         <f>D9*(C2*VLOOKUP(B2, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C3*VLOOKUP(B3, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C4*VLOOKUP(B4, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C5*VLOOKUP(B5, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
         <v>0.19710482450933728</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G9" s="2">
+        <f>F9*(F15*VLOOKUP(B15, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + F16*VLOOKUP(B16, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + F17*VLOOKUP(B17, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + F18*VLOOKUP(B18, 'Match Predictions'!$D$157:$Y$187, 21, FALSE)+(F21*VLOOKUP(B21, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + F22*VLOOKUP(B22, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + F23*VLOOKUP(B23, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + F24*VLOOKUP(B24, 'Match Predictions'!$D$157:$Y$187, 21, FALSE)))</f>
+        <v>0.1129438694070725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2">
@@ -80307,14 +80295,16 @@
         <f>D10*(C2*VLOOKUP(B2, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C3*VLOOKUP(B3, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C4*VLOOKUP(B4, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C5*VLOOKUP(B5, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
         <v>0.14944151217706397</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G10" s="2">
+        <f>F10*(F15*VLOOKUP(B15,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F16*VLOOKUP(B16,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F17*VLOOKUP(B17,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F18*VLOOKUP(B18,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F21*VLOOKUP(B21,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F22*VLOOKUP(B22,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F23*VLOOKUP(B23,'Match Predictions'!$D$188:$Y$218,21,FALSE)+F24*VLOOKUP(B24,'Match Predictions'!$D$188:$Y$218,21,FALSE))</f>
+        <v>6.4794329215562288E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2">
@@ -80331,11 +80321,12 @@
         <f>D11*(C2*VLOOKUP(B2, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C3*VLOOKUP(B3, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C4*VLOOKUP(B4, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C5*VLOOKUP(B5, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
         <v>9.830728795157638E-2</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
+      <c r="G11" s="2">
+        <f>D11*(F15*VLOOKUP(B15, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + F16*VLOOKUP(B16, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + F17*VLOOKUP(B17, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + F18*VLOOKUP(B18, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) +F21*VLOOKUP(B21, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + F22*VLOOKUP(B22, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + F23*VLOOKUP(B23, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + F24*VLOOKUP(B24, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
+        <v>6.8820902312447141E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <f t="shared" ref="C12" si="2">SUM(C8:C11)</f>
         <v>0.99999999999999989</v>
@@ -80352,11 +80343,8 @@
         <f>SUM(F8:F11)</f>
         <v>0.61657109412329869</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -80364,23 +80352,21 @@
         <f>F12+F6</f>
         <v>1</v>
       </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="2">
@@ -80396,13 +80382,12 @@
         <f>D15*(C21*VLOOKUP(B21, 'Match Predictions'!$D$374:$Y$404, 21, FALSE) + C22*VLOOKUP(B22, 'Match Predictions'!$D$374:$Y$404, 21, FALSE) + C23*VLOOKUP(B23, 'Match Predictions'!$D$374:$Y$404, 21, FALSE) + C24*VLOOKUP(B24, 'Match Predictions'!$D$374:$Y$404, 21, FALSE))</f>
         <v>0.16076488529114677</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2">
@@ -80418,13 +80403,12 @@
         <f>D16*(C21*VLOOKUP(B21, 'Match Predictions'!$D$405:$Y$435, 21, FALSE) + C22*VLOOKUP(B22, 'Match Predictions'!$D$405:$Y$435, 21, FALSE) + C23*VLOOKUP(B23, 'Match Predictions'!$D$405:$Y$435, 21, FALSE) + C24*VLOOKUP(B24, 'Match Predictions'!$D$405:$Y$435, 21, FALSE))</f>
         <v>7.7007561860349821E-2</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="2">
@@ -80440,13 +80424,12 @@
         <f>D17*(C21*VLOOKUP(B21, 'Match Predictions'!$D$436:$Y$466, 21, FALSE) + C22*VLOOKUP(B22, 'Match Predictions'!$D$436:$Y$466, 21, FALSE) + C23*VLOOKUP(B23, 'Match Predictions'!$D$436:$Y$466, 21, FALSE) + C24*VLOOKUP(B24, 'Match Predictions'!$D$436:$Y$466, 21, FALSE))</f>
         <v>0.13039429387229698</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2">
@@ -80462,10 +80445,8 @@
         <f>D18*(C21*VLOOKUP(B21, 'Match Predictions'!$D$467:$Y$497, 21, FALSE) + C22*VLOOKUP(B22, 'Match Predictions'!$D$467:$Y$497, 21, FALSE) + C23*VLOOKUP(B23, 'Match Predictions'!$D$467:$Y$497, 21, FALSE) + C24*VLOOKUP(B24, 'Match Predictions'!$D$467:$Y$497, 21, FALSE))</f>
         <v>5.8894366790018207E-2</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C19" s="2">
         <f t="shared" ref="C19" si="5">SUM(C15:C18)</f>
         <v>1</v>
@@ -80482,25 +80463,21 @@
         <f>SUM(F15:F18)</f>
         <v>0.42706110781381174</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="2">
@@ -80516,14 +80493,12 @@
         <f>C21*(D15*VLOOKUP(B15, 'Match Predictions'!$D$250:$Y$280, 21, FALSE) + D16*VLOOKUP(B16, 'Match Predictions'!$D$250:$Y$280, 21, FALSE) + D17*VLOOKUP(B17, 'Match Predictions'!$D$250:$Y$280, 21, FALSE) + D18*VLOOKUP(B18, 'Match Predictions'!$D$250:$Y$280, 21, FALSE))</f>
         <v>0.33449459367330364</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="2">
@@ -80539,14 +80514,12 @@
         <f>C22*(D15*VLOOKUP(B15, 'Match Predictions'!$D$281:$Y$311, 21, FALSE) + D16*VLOOKUP(B16, 'Match Predictions'!$D$281:$Y$311, 21, FALSE) + D17*VLOOKUP(B17, 'Match Predictions'!$D$281:$Y$311, 21, FALSE) + D18*VLOOKUP(B18, 'Match Predictions'!$D$281:$Y$311, 21, FALSE))</f>
         <v>1.3019724261565491E-2</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="2">
@@ -80562,15 +80535,12 @@
         <f>C23*(D15*VLOOKUP(B15, 'Match Predictions'!$D$312:$Y$342, 21, FALSE) + D16*VLOOKUP(B16, 'Match Predictions'!$D$312:$Y$342, 21, FALSE) + D17*VLOOKUP(B17, 'Match Predictions'!$D$312:$Y$342, 21, FALSE) + D18*VLOOKUP(B18, 'Match Predictions'!$D$312:$Y$342, 21, FALSE))</f>
         <v>0.10772527160242208</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="2">
@@ -80586,12 +80556,8 @@
         <f>C24*(D15*VLOOKUP(B15, 'Match Predictions'!$D$343:$Y$373, 21, FALSE) + D16*VLOOKUP(B16, 'Match Predictions'!$D$343:$Y$373, 21, FALSE) + D17*VLOOKUP(B17, 'Match Predictions'!$D$343:$Y$373, 21, FALSE) + D18*VLOOKUP(B18, 'Match Predictions'!$D$343:$Y$373, 21, FALSE))</f>
         <v>0.11769930264889697</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
       <c r="C25" s="2">
         <f t="shared" ref="C25" si="8">SUM(C21:C24)</f>
         <v>1</v>
@@ -80608,12 +80574,8 @@
         <f>SUM(F21:F24)</f>
         <v>0.57293889218618821</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -80621,41 +80583,48 @@
         <f>F25+F19</f>
         <v>1</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
+      <c r="G26" s="2">
+        <f>SUM(G2:G25)</f>
+        <v>0.46725216256576546</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="2">
@@ -80671,15 +80640,12 @@
         <f>C29*(D35*VLOOKUP(B35, 'Match Predictions'!$D$498:$Y$528, 21, FALSE) + D36*VLOOKUP(B36, 'Match Predictions'!$D$498:$Y$528, 21, FALSE) + D37*VLOOKUP(B37, 'Match Predictions'!$D$498:$Y$528, 21, FALSE) + D38*VLOOKUP(B38, 'Match Predictions'!$D$498:$Y$528, 21, FALSE))</f>
         <v>0.40982891605077865</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="2">
@@ -80695,15 +80661,12 @@
         <f>C30*(D35*VLOOKUP(B35, 'Match Predictions'!$D$529:$Y$559, 21, FALSE) + D36*VLOOKUP(B36, 'Match Predictions'!$D$529:$Y$559, 21, FALSE) + D37*VLOOKUP(B37, 'Match Predictions'!$D$529:$Y$559, 21, FALSE) + D38*VLOOKUP(B38, 'Match Predictions'!$D$529:$Y$559, 21, FALSE))</f>
         <v>4.7459313752099462E-2</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="2">
@@ -80719,15 +80682,12 @@
         <f>C31*(D35*VLOOKUP(B35, 'Match Predictions'!$D$560:$Y$590, 21, FALSE) + D36*VLOOKUP(B36, 'Match Predictions'!$D$560:$Y$590, 21, FALSE) + D37*VLOOKUP(B37, 'Match Predictions'!$D$560:$Y$590, 21, FALSE) + D38*VLOOKUP(B38, 'Match Predictions'!$D$560:$Y$590, 21, FALSE))</f>
         <v>4.9053345052754702E-2</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>111</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="2">
@@ -80743,10 +80703,8 @@
         <f>C32*(D35*VLOOKUP(B35, 'Match Predictions'!$D$591:$Y$621, 21, FALSE) + D36*VLOOKUP(B36, 'Match Predictions'!$D$591:$Y$621, 21, FALSE) + D37*VLOOKUP(B37, 'Match Predictions'!$D$591:$Y$621, 21, FALSE) + D38*VLOOKUP(B38, 'Match Predictions'!$D$591:$Y$621, 21, FALSE))</f>
         <v>4.0724358894762828E-2</v>
       </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C33" s="2">
         <f t="shared" ref="C33" si="11">SUM(C29:C32)</f>
         <v>1</v>
@@ -80763,23 +80721,21 @@
         <f>SUM(F29:F32)</f>
         <v>0.54706593375039558</v>
       </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="2">
@@ -80795,13 +80751,12 @@
         <f>D35*(C29*VLOOKUP(B29, 'Match Predictions'!$D$622:$Y$652, 21, FALSE) + C30*VLOOKUP(B30, 'Match Predictions'!$D$622:$Y$652, 21, FALSE) + C31*VLOOKUP(B31, 'Match Predictions'!$D$622:$Y$652, 21, FALSE) + C32*VLOOKUP(B32, 'Match Predictions'!$D$622:$Y$652, 21, FALSE))</f>
         <v>0.16365602070302113</v>
       </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="2">
@@ -80817,15 +80772,12 @@
         <f>D36*(C29*VLOOKUP(B29, 'Match Predictions'!$D$653:$Y$683, 21, FALSE) + C30*VLOOKUP(B30, 'Match Predictions'!$D$653:$Y$683, 21, FALSE) + C31*VLOOKUP(B31, 'Match Predictions'!$D$653:$Y$683, 21, FALSE) + C32*VLOOKUP(B32, 'Match Predictions'!$D$653:$Y$683, 21, FALSE))</f>
         <v>0.11754898664532555</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="2">
@@ -80841,15 +80793,12 @@
         <f>D37*(C29*VLOOKUP(B29, 'Match Predictions'!$D$684:$Y$714, 21, FALSE) + C30*VLOOKUP(B30, 'Match Predictions'!$D$684:$Y$714, 21, FALSE) + C31*VLOOKUP(B31, 'Match Predictions'!$D$684:$Y$714, 21, FALSE) + C32*VLOOKUP(B32, 'Match Predictions'!$D$684:$Y$714, 21, FALSE))</f>
         <v>0.14478722705625574</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="2">
@@ -80865,12 +80814,8 @@
         <f>D38*(C29*VLOOKUP(B29, 'Match Predictions'!$D$715:$Y$745, 21, FALSE) + C30*VLOOKUP(B30, 'Match Predictions'!$D$715:$Y$745, 21, FALSE) + C31*VLOOKUP(B31, 'Match Predictions'!$D$715:$Y$745, 21, FALSE) + C32*VLOOKUP(B32, 'Match Predictions'!$D$715:$Y$745, 21, FALSE))</f>
         <v>2.6941831845001936E-2</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C39" s="2">
         <f t="shared" ref="C39" si="14">SUM(C35:C38)</f>
         <v>1</v>
@@ -80887,12 +80832,8 @@
         <f>SUM(F35:F38)</f>
         <v>0.45293406624960436</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -80900,27 +80841,21 @@
         <f>F39+F33</f>
         <v>1</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B41" s="3" t="s">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="2">
@@ -80936,15 +80871,12 @@
         <f>D42*(C48*VLOOKUP(B48, 'Match Predictions'!$D$870:$Y$900, 21, FALSE) + C49*VLOOKUP(B49, 'Match Predictions'!$D$870:$Y$900, 21, FALSE) + C50*VLOOKUP(B50, 'Match Predictions'!$D$870:$Y$900, 21, FALSE) + C51*VLOOKUP(B51, 'Match Predictions'!$D$870:$Y$900, 21, FALSE))</f>
         <v>0.13408967121649551</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="2">
@@ -80960,15 +80892,12 @@
         <f>D43*(C48*VLOOKUP(B48, 'Match Predictions'!$D$901:$Y$931, 21, FALSE) + C49*VLOOKUP(B49, 'Match Predictions'!$D$901:$Y$931, 21, FALSE) + C50*VLOOKUP(B50, 'Match Predictions'!$D$901:$Y$931, 21, FALSE) + C51*VLOOKUP(B51, 'Match Predictions'!$D$901:$Y$931, 21, FALSE))</f>
         <v>7.3471552176513522E-2</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" t="s">
         <v>44</v>
       </c>
       <c r="C44" s="2">
@@ -80984,15 +80913,12 @@
         <f>D44*(C48*VLOOKUP(B48, 'Match Predictions'!$D$932:$Y$962, 21, FALSE) + C49*VLOOKUP(B49, 'Match Predictions'!$D$932:$Y$962, 21, FALSE) + C50*VLOOKUP(B50, 'Match Predictions'!$D$932:$Y$962, 21, FALSE) + C51*VLOOKUP(B51, 'Match Predictions'!$D$932:$Y$962, 21, FALSE))</f>
         <v>0.16111682524421317</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="2">
@@ -81008,12 +80934,8 @@
         <f>D45*(C48*VLOOKUP(B48, 'Match Predictions'!$D$963:$Y$993, 21, FALSE) + C49*VLOOKUP(B49, 'Match Predictions'!$D$963:$Y$993, 21, FALSE) + C50*VLOOKUP(B50, 'Match Predictions'!$D$963:$Y$993, 21, FALSE) + C51*VLOOKUP(B51, 'Match Predictions'!$D$963:$Y$993, 21, FALSE))</f>
         <v>5.3859651886156448E-2</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C46" s="2">
         <f t="shared" ref="C46" si="17">SUM(C42:C45)</f>
         <v>1</v>
@@ -81030,27 +80952,21 @@
         <f>SUM(F42:F45)</f>
         <v>0.42253770052337863</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="3" t="s">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>89</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
         <v>36</v>
       </c>
       <c r="C48" s="2">
@@ -81066,15 +80982,12 @@
         <f>C48*(D42*VLOOKUP(B42, 'Match Predictions'!$D$746:$Y$776, 21, FALSE) + D43*VLOOKUP(B43, 'Match Predictions'!$D$746:$Y$776, 21, FALSE) + D44*VLOOKUP(B44, 'Match Predictions'!$D$746:$Y$776, 21, FALSE) + D45*VLOOKUP(B45, 'Match Predictions'!$D$746:$Y$776, 21, FALSE))</f>
         <v>0.34451480239659688</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" t="s">
         <v>38</v>
       </c>
       <c r="C49" s="2">
@@ -81090,15 +81003,12 @@
         <f>C49*(D42*VLOOKUP(B42, 'Match Predictions'!$D$777:$Y$807, 21, FALSE) + D43*VLOOKUP(B43, 'Match Predictions'!$D$777:$Y$807, 21, FALSE) + D44*VLOOKUP(B44, 'Match Predictions'!$D$777:$Y$807, 21, FALSE) + D45*VLOOKUP(B45, 'Match Predictions'!$D$777:$Y$807, 21, FALSE))</f>
         <v>1.3699914933414784E-2</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>118</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" t="s">
         <v>39</v>
       </c>
       <c r="C50" s="2">
@@ -81114,15 +81024,12 @@
         <f>C50*(D42*VLOOKUP(B42, 'Match Predictions'!$D$808:$Y$838, 21, FALSE) + D43*VLOOKUP(B43, 'Match Predictions'!$D$808:$Y$838, 21, FALSE) + D44*VLOOKUP(B44, 'Match Predictions'!$D$808:$Y$838, 21, FALSE) + D45*VLOOKUP(B45, 'Match Predictions'!$D$808:$Y$838, 21, FALSE))</f>
         <v>1.882375226959334E-2</v>
       </c>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" t="s">
         <v>40</v>
       </c>
       <c r="C51" s="2">
@@ -81138,12 +81045,8 @@
         <f>C51*(D42*VLOOKUP(B42, 'Match Predictions'!$D$839:$Y$869, 21, FALSE) + D43*VLOOKUP(B43, 'Match Predictions'!$D$839:$Y$869, 21, FALSE) + D44*VLOOKUP(B44, 'Match Predictions'!$D$839:$Y$869, 21, FALSE) + D45*VLOOKUP(B45, 'Match Predictions'!$D$839:$Y$869, 21, FALSE))</f>
         <v>0.20042382987701626</v>
       </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="2"/>
       <c r="C52" s="2">
         <f t="shared" ref="C52" si="20">SUM(C48:C51)</f>
         <v>1</v>
@@ -81160,12 +81063,8 @@
         <f>SUM(F48:F51)</f>
         <v>0.5774622994766212</v>
       </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -81173,44 +81072,44 @@
         <f>F52+F46</f>
         <v>0.99999999999999978</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G55" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H55" s="4" t="s">
+      <c r="H55" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I55" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" t="s">
         <v>11</v>
       </c>
       <c r="C56" s="2">
@@ -81227,15 +81126,12 @@
         <f>C56*(D62*VLOOKUP(B62, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + D63*VLOOKUP(B63, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + D64*VLOOKUP(B64, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + D65*VLOOKUP(B65, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
         <v>0.16468071187978453</v>
       </c>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="2">
@@ -81252,15 +81148,12 @@
         <f>C57*(D62*VLOOKUP(B62, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + D63*VLOOKUP(B63, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + D64*VLOOKUP(B64, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + D65*VLOOKUP(B65, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
         <v>0.34628468159497033</v>
       </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="2">
@@ -81277,15 +81170,12 @@
         <f>C58*(D62*VLOOKUP(B62, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + D63*VLOOKUP(B63, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + D64*VLOOKUP(B64, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + D65*VLOOKUP(B65, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
         <v>0.11971051370413367</v>
       </c>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>107</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="2">
@@ -81302,12 +81192,8 @@
         <f>C59*(D62*VLOOKUP(B62, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + D63*VLOOKUP(B63, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + D64*VLOOKUP(B64, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + D65*VLOOKUP(B65, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
         <v>6.2615843643042735E-2</v>
       </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B60" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C60" s="2">
         <f t="shared" ref="C60" si="23">SUM(C56:C59)</f>
         <v>0.99999999999999989</v>
@@ -81324,27 +81210,21 @@
         <f>SUM(F56:F59)</f>
         <v>0.69329175082193129</v>
       </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B61" s="3" t="s">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-    </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>103</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="2">
@@ -81361,15 +81241,12 @@
         <f>D62*(C56*VLOOKUP(B56, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C57*VLOOKUP(B57, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C58*VLOOKUP(B58, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C59*VLOOKUP(B59, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
         <v>8.2284952200555594E-2</v>
       </c>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-    </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="2">
@@ -81386,15 +81263,12 @@
         <f>D63*(C56*VLOOKUP(B56, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C57*VLOOKUP(B57, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C58*VLOOKUP(B58, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C59*VLOOKUP(B59, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
         <v>3.3837264602812923E-2</v>
       </c>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-    </row>
-    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>101</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="2">
@@ -81411,15 +81285,12 @@
         <f>D64*(C56*VLOOKUP(B56, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C57*VLOOKUP(B57, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C58*VLOOKUP(B58, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C59*VLOOKUP(B59, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
         <v>7.5444129042134156E-2</v>
       </c>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>100</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" t="s">
         <v>10</v>
       </c>
       <c r="C65" s="2">
@@ -81436,12 +81307,8 @@
         <f>D65*(C56*VLOOKUP(B56, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C57*VLOOKUP(B57, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C58*VLOOKUP(B58, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C59*VLOOKUP(B59, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
         <v>0.11514190333256598</v>
       </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B66" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C66" s="2">
         <f t="shared" ref="C66" si="27">SUM(C62:C65)</f>
         <v>1</v>
@@ -81458,37 +81325,30 @@
         <f>SUM(F62:F65)</f>
         <v>0.30670824917806866</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
       <c r="F67" s="2">
         <f>F60+F66</f>
         <v>1</v>
       </c>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B68" s="3" t="s">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
         <v>80</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="K68" s="4"/>
-    </row>
-    <row r="69" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>99</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" t="s">
         <v>16</v>
       </c>
       <c r="C69" s="2">
@@ -81504,20 +81364,12 @@
         <f>D69*(C75*VLOOKUP(B75, 'Match Predictions'!$D$250:$Y$280, 21, FALSE) + C76*VLOOKUP(B76, 'Match Predictions'!$D$250:$Y$280, 21, FALSE) + C77*VLOOKUP(B77, 'Match Predictions'!$D$250:$Y$280, 21, FALSE) + C78*VLOOKUP(B78, 'Match Predictions'!$D$250:$Y$280, 21, FALSE))</f>
         <v>0.16201085473999247</v>
       </c>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-    </row>
-    <row r="70" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" t="s">
         <v>18</v>
       </c>
       <c r="C70" s="2">
@@ -81533,20 +81385,12 @@
         <f>D70*(C75*VLOOKUP(B75, 'Match Predictions'!$D$281:$Y$311, 21, FALSE) + C76*VLOOKUP(B76, 'Match Predictions'!$D$281:$Y$311, 21, FALSE) + C77*VLOOKUP(B77, 'Match Predictions'!$D$281:$Y$311, 21, FALSE) + C78*VLOOKUP(B78, 'Match Predictions'!$D$281:$Y$311, 21, FALSE))</f>
         <v>2.5997008486715663E-2</v>
       </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-    </row>
-    <row r="71" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>97</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" t="s">
         <v>19</v>
       </c>
       <c r="C71" s="2">
@@ -81562,20 +81406,12 @@
         <f>D71*(C75*VLOOKUP(B75, 'Match Predictions'!$D$312:$Y$342, 21, FALSE) + C76*VLOOKUP(B76, 'Match Predictions'!$D$312:$Y$342, 21, FALSE) + C77*VLOOKUP(B77, 'Match Predictions'!$D$312:$Y$342, 21, FALSE) + C78*VLOOKUP(B78, 'Match Predictions'!$D$312:$Y$342, 21, FALSE))</f>
         <v>0.12265719394605847</v>
       </c>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-    </row>
-    <row r="72" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" t="s">
         <v>20</v>
       </c>
       <c r="C72" s="2">
@@ -81591,17 +81427,8 @@
         <f>D72*(C75*VLOOKUP(B75, 'Match Predictions'!$D$343:$Y$373, 21, FALSE) + C76*VLOOKUP(B76, 'Match Predictions'!$D$343:$Y$373, 21, FALSE) + C77*VLOOKUP(B77, 'Match Predictions'!$D$343:$Y$373, 21, FALSE) + C78*VLOOKUP(B78, 'Match Predictions'!$D$343:$Y$373, 21, FALSE))</f>
         <v>0.13326050936353673</v>
       </c>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B73" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C73" s="2">
         <f t="shared" ref="C73" si="30">SUM(C69:C72)</f>
         <v>1</v>
@@ -81618,37 +81445,21 @@
         <f>SUM(F69:F72)</f>
         <v>0.44392556653630333</v>
       </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-      <c r="O73" s="2"/>
-    </row>
-    <row r="74" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B74" s="3" t="s">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>81</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-      <c r="N74" s="2"/>
-      <c r="O74" s="2"/>
-    </row>
-    <row r="75" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>93</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" t="s">
         <v>21</v>
       </c>
       <c r="C75" s="2">
@@ -81664,20 +81475,12 @@
         <f>C75*(D69*VLOOKUP(B69, 'Match Predictions'!$D$374:$Y$404, 21, FALSE) + D70*VLOOKUP(B70, 'Match Predictions'!$D$374:$Y$404, 21, FALSE) + D71*VLOOKUP(B71, 'Match Predictions'!$D$374:$Y$404, 21, FALSE) + D72*VLOOKUP(B72, 'Match Predictions'!$D$374:$Y$404, 21, FALSE))</f>
         <v>0.35672635800721691</v>
       </c>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
-      <c r="O75" s="2"/>
-    </row>
-    <row r="76" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>94</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" t="s">
         <v>23</v>
       </c>
       <c r="C76" s="2">
@@ -81693,20 +81496,12 @@
         <f>C76*(D69*VLOOKUP(B69, 'Match Predictions'!$D$405:$Y$435, 21, FALSE) + D70*VLOOKUP(B70, 'Match Predictions'!$D$405:$Y$435, 21, FALSE) + D71*VLOOKUP(B71, 'Match Predictions'!$D$405:$Y$435, 21, FALSE) + D72*VLOOKUP(B72, 'Match Predictions'!$D$405:$Y$435, 21, FALSE))</f>
         <v>5.1928950156461338E-2</v>
       </c>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-    </row>
-    <row r="77" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>95</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" t="s">
         <v>24</v>
       </c>
       <c r="C77" s="2">
@@ -81722,20 +81517,12 @@
         <f>C77*(D69*VLOOKUP(B69, 'Match Predictions'!$D$436:$Y$466, 21, FALSE) + D70*VLOOKUP(B70, 'Match Predictions'!$D$436:$Y$466, 21, FALSE) + D71*VLOOKUP(B71, 'Match Predictions'!$D$436:$Y$466, 21, FALSE) + D72*VLOOKUP(B72, 'Match Predictions'!$D$436:$Y$466, 21, FALSE))</f>
         <v>0.11140287429207224</v>
       </c>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-    </row>
-    <row r="78" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>96</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" t="s">
         <v>25</v>
       </c>
       <c r="C78" s="2">
@@ -81751,17 +81538,8 @@
         <f>C78*(D69*VLOOKUP(B69, 'Match Predictions'!$D$467:$Y$497, 21, FALSE) + D70*VLOOKUP(B70, 'Match Predictions'!$D$467:$Y$497, 21, FALSE) + D71*VLOOKUP(B71, 'Match Predictions'!$D$467:$Y$497, 21, FALSE) + D72*VLOOKUP(B72, 'Match Predictions'!$D$467:$Y$497, 21, FALSE))</f>
         <v>3.6016251007946219E-2</v>
       </c>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-    </row>
-    <row r="79" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B79" s="3"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C79" s="2">
         <f t="shared" ref="C79" si="33">SUM(C75:C78)</f>
         <v>1</v>
@@ -81778,17 +81556,8 @@
         <f>SUM(F75:F78)</f>
         <v>0.55607443346369667</v>
       </c>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B80" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -81796,14 +81565,6 @@
         <f>F79+F73</f>
         <v>1</v>
       </c>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" s="2"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C81" s="2"/>
@@ -81812,28 +81573,28 @@
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B82" s="4" t="s">
+      <c r="B82" t="s">
         <v>90</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="F82" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H82" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="I82" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -81841,256 +81602,216 @@
       <c r="A83" t="s">
         <v>112</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>6</v>
+      <c r="B83" t="s">
+        <v>31</v>
       </c>
       <c r="C83" s="2">
-        <v>0.21679999999999999</v>
+        <v>0.61929999999999996</v>
       </c>
       <c r="D83" s="2">
-        <f>E83-C83</f>
-        <v>0.28260000000000002</v>
+        <v>0.2419</v>
       </c>
       <c r="E83" s="2">
-        <v>0.49940000000000001</v>
+        <v>0.86119999999999997</v>
       </c>
       <c r="F83" s="2">
-        <f>C83*(D89*VLOOKUP(B89, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
-        <v>7.0158613114117196E-2</v>
-      </c>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
+        <f>C83*(D89*VLOOKUP(B89, 'Match Predictions'!$D$622:$Y$652, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$622:$Y$652, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$622:$Y$652, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$622:$Y$652, 21, FALSE))</f>
+        <v>0.48085403638794472</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>8</v>
+      <c r="B84" t="s">
+        <v>33</v>
       </c>
       <c r="C84" s="2">
-        <v>0.1036</v>
+        <v>0.14860000000000001</v>
       </c>
       <c r="D84" s="2">
-        <f t="shared" ref="D84:D86" si="36">E84-C84</f>
-        <v>0.18679999999999999</v>
+        <v>0.29559999999999997</v>
       </c>
       <c r="E84" s="2">
-        <v>0.29039999999999999</v>
+        <v>0.44419999999999998</v>
       </c>
       <c r="F84" s="2">
-        <f>C84*(D89*VLOOKUP(B89, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
-        <v>2.1560551582548132E-2</v>
-      </c>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
+        <f>C84*(D89*VLOOKUP(B89, 'Match Predictions'!$D$653:$Y$683, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D653:$Y$683, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D653:$Y$683, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D653:$Y$683, 21, FALSE))</f>
+        <v>7.7514812401040287E-2</v>
+      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>9</v>
+      <c r="B85" t="s">
+        <v>34</v>
       </c>
       <c r="C85" s="2">
-        <v>0.18179999999999999</v>
+        <v>0.1946</v>
       </c>
       <c r="D85" s="2">
-        <f t="shared" si="36"/>
-        <v>0.26580000000000004</v>
+        <v>0.33860000000000001</v>
       </c>
       <c r="E85" s="2">
-        <v>0.4476</v>
+        <v>0.53320000000000001</v>
       </c>
       <c r="F85" s="2">
-        <f>C85*(D89*VLOOKUP(B89, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
-        <v>5.7137825352393028E-2</v>
-      </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
+        <f>C85*(D89*VLOOKUP(B89, 'Match Predictions'!$D$684:$Y$714, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$684:$Y$714, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$684:$Y$714, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$684:$Y$714, 21, FALSE))</f>
+        <v>0.10765804549554522</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>115</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>10</v>
+      <c r="B86" t="s">
+        <v>35</v>
       </c>
       <c r="C86" s="2">
-        <v>0.49780000000000002</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D86" s="2">
-        <f t="shared" si="36"/>
-        <v>0.26479999999999992</v>
+        <v>0.12389999999999998</v>
       </c>
       <c r="E86" s="2">
-        <v>0.76259999999999994</v>
+        <v>0.16139999999999999</v>
       </c>
       <c r="F86" s="2">
-        <f>C86*(D89*VLOOKUP(B89, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
-        <v>0.23457191582764303</v>
-      </c>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
+        <f>C86*(D89*VLOOKUP(B89, 'Match Predictions'!$D$715:$Y$745, 21, FALSE) + D90*VLOOKUP(B90, 'Match Predictions'!$D$715:$Y$745, 21, FALSE) + D91*VLOOKUP(B91, 'Match Predictions'!$D$715:$Y$745, 21, FALSE) + D92*VLOOKUP(B92, 'Match Predictions'!$D$715:$Y$745, 21, FALSE))</f>
+        <v>1.1771860248917606E-2</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B87" s="2"/>
       <c r="C87" s="2">
-        <f t="shared" ref="C87" si="37">SUM(C83:C86)</f>
+        <f t="shared" ref="C87" si="36">SUM(C83:C86)</f>
         <v>1</v>
       </c>
       <c r="D87" s="2">
-        <f t="shared" ref="D87" si="38">SUM(D83:D86)</f>
+        <f t="shared" ref="D87" si="37">SUM(D83:D86)</f>
         <v>1</v>
       </c>
       <c r="E87" s="2">
-        <f t="shared" ref="E87" si="39">SUM(E83:E86)</f>
+        <f t="shared" ref="E87" si="38">SUM(E83:E86)</f>
         <v>2</v>
       </c>
       <c r="F87" s="2">
         <f>SUM(F83:F86)</f>
-        <v>0.38342890587670142</v>
-      </c>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
+        <v>0.67779875453344784</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B88" s="4" t="s">
+      <c r="B88" t="s">
         <v>91</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>11</v>
+      <c r="B89" t="s">
+        <v>26</v>
       </c>
       <c r="C89" s="2">
-        <v>0.24510000000000001</v>
+        <v>0.62909999999999999</v>
       </c>
       <c r="D89" s="2">
-        <f>E89-C89</f>
-        <v>0.27490000000000003</v>
+        <v>0.21870000000000001</v>
       </c>
       <c r="E89" s="2">
-        <v>0.52</v>
+        <v>0.8478</v>
       </c>
       <c r="F89" s="2">
-        <f>D89*(C83*VLOOKUP(B83, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
-        <v>0.17171746948532104</v>
-      </c>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
+        <f>D89*(C83*VLOOKUP(B83, 'Match Predictions'!$D$498:$Y$528, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$498:$Y$528, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$498:$Y$528, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$498:$Y$528, 21, FALSE))</f>
+        <v>0.11562662551930974</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>109</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>13</v>
+      <c r="B90" t="s">
+        <v>28</v>
       </c>
       <c r="C90" s="2">
-        <v>0.44869999999999999</v>
+        <v>0.12709999999999999</v>
       </c>
       <c r="D90" s="2">
-        <f>E90-C90</f>
-        <v>0.26890000000000003</v>
+        <v>0.26519999999999999</v>
       </c>
       <c r="E90" s="2">
-        <v>0.71760000000000002</v>
+        <v>0.39229999999999998</v>
       </c>
       <c r="F90" s="2">
-        <f>D90*(C83*VLOOKUP(B83, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
-        <v>0.19710482450933728</v>
-      </c>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
+        <f>D90*(C83*VLOOKUP(B83, 'Match Predictions'!$D$529:$Y$559, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$529:$Y$559, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$529:$Y$559, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$529:$Y$559, 21, FALSE))</f>
+        <v>7.0604740347875949E-2</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>110</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>14</v>
+      <c r="B91" t="s">
+        <v>29</v>
       </c>
       <c r="C91" s="2">
-        <v>0.19</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="D91" s="2">
-        <f>E91-C91</f>
-        <v>0.2555</v>
+        <v>0.27369999999999994</v>
       </c>
       <c r="E91" s="2">
-        <v>0.44550000000000001</v>
+        <v>0.40039999999999998</v>
       </c>
       <c r="F91" s="2">
-        <f>D91*(C83*VLOOKUP(B83, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
-        <v>0.14944151217706397</v>
-      </c>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+        <f>D91*(C83*VLOOKUP(B83, 'Match Predictions'!$D$560:$Y$590, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$560:$Y$590, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$560:$Y$590, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$560:$Y$590, 21, FALSE))</f>
+        <v>7.7883675703194793E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>111</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>15</v>
+      <c r="B92" t="s">
+        <v>30</v>
       </c>
       <c r="C92" s="2">
-        <v>0.1162</v>
+        <v>0.1171</v>
       </c>
       <c r="D92" s="2">
-        <f>E92-C92</f>
-        <v>0.20070000000000002</v>
+        <v>0.2424</v>
       </c>
       <c r="E92" s="2">
-        <v>0.31690000000000002</v>
+        <v>0.35949999999999999</v>
       </c>
       <c r="F92" s="2">
-        <f>D92*(C83*VLOOKUP(B83, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
-        <v>9.830728795157638E-2</v>
-      </c>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
+        <f>D92*(C83*VLOOKUP(B83, 'Match Predictions'!$D$591:$Y$621, 21, FALSE) + C84*VLOOKUP(B84, 'Match Predictions'!$D$591:$Y$621, 21, FALSE) + C85*VLOOKUP(B85, 'Match Predictions'!$D$591:$Y$621, 21, FALSE) + C86*VLOOKUP(B86, 'Match Predictions'!$D$591:$Y$621, 21, FALSE))</f>
+        <v>5.8086203896171723E-2</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B93" s="2"/>
       <c r="C93" s="2">
-        <f t="shared" ref="C93" si="40">SUM(C89:C92)</f>
-        <v>0.99999999999999989</v>
+        <f t="shared" ref="C93" si="39">SUM(C89:C92)</f>
+        <v>1</v>
       </c>
       <c r="D93" s="2">
-        <f t="shared" ref="D93" si="41">SUM(D89:D92)</f>
-        <v>1.0000000000000002</v>
+        <f t="shared" ref="D93" si="40">SUM(D89:D92)</f>
+        <v>1</v>
       </c>
       <c r="E93" s="2">
-        <f t="shared" ref="E93" si="42">SUM(E89:E92)</f>
-        <v>2</v>
+        <f t="shared" ref="E93" si="41">SUM(E89:E92)</f>
+        <v>1.9999999999999998</v>
       </c>
       <c r="F93" s="2">
         <f>SUM(F89:F92)</f>
-        <v>0.61657109412329869</v>
-      </c>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
+        <v>0.32220124546655216</v>
+      </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -82098,267 +81819,230 @@
         <f>F93+F87</f>
         <v>1</v>
       </c>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B95" s="4" t="s">
+      <c r="B95" t="s">
         <v>84</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>116</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>6</v>
+      <c r="B96" t="s">
+        <v>36</v>
       </c>
       <c r="C96" s="2">
-        <v>0.21679999999999999</v>
+        <v>0.5323</v>
       </c>
       <c r="D96" s="2">
-        <f>E96-C96</f>
-        <v>0.28260000000000002</v>
+        <v>0.29920000000000002</v>
       </c>
       <c r="E96" s="2">
-        <v>0.49940000000000001</v>
+        <v>0.83150000000000002</v>
       </c>
       <c r="F96" s="2">
-        <f>D96*(C102*VLOOKUP(B102, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$2:$Y$32, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$2:$Y$32, 21, FALSE))</f>
-        <v>8.2284952200555594E-2</v>
-      </c>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+        <f>D96*(C102*VLOOKUP(B102, 'Match Predictions'!$D$746:$Y$776, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$746:$Y$776, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$746:$Y$776, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$746:$Y$776, 21, FALSE))</f>
+        <v>0.1797388345047907</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>117</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>8</v>
+      <c r="B97" t="s">
+        <v>38</v>
       </c>
       <c r="C97" s="2">
-        <v>0.1036</v>
+        <v>5.4899999999999997E-2</v>
       </c>
       <c r="D97" s="2">
-        <f t="shared" ref="D97:D99" si="43">E97-C97</f>
-        <v>0.18679999999999999</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="E97" s="2">
-        <v>0.29039999999999999</v>
+        <v>0.20050000000000001</v>
       </c>
       <c r="F97" s="2">
-        <f>D97*(C102*VLOOKUP(B102, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$33:$Y$63, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$33:$Y$63, 21, FALSE))</f>
-        <v>3.3837264602812923E-2</v>
-      </c>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+        <f>D97*(C102*VLOOKUP(B102, 'Match Predictions'!$D$777:$Y$807, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$777:$Y$807, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$777:$Y$807, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$777:$Y$807, 21, FALSE))</f>
+        <v>3.0928184925798435E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>9</v>
+      <c r="B98" t="s">
+        <v>39</v>
       </c>
       <c r="C98" s="2">
-        <v>0.18179999999999999</v>
+        <v>6.8099999999999994E-2</v>
       </c>
       <c r="D98" s="2">
-        <f t="shared" si="43"/>
-        <v>0.26580000000000004</v>
+        <v>0.1676</v>
       </c>
       <c r="E98" s="2">
-        <v>0.4476</v>
+        <v>0.23569999999999999</v>
       </c>
       <c r="F98" s="2">
-        <f>D98*(C102*VLOOKUP(B102, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$64:$Y$94, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$64:$Y$94, 21, FALSE))</f>
-        <v>7.5444129042134156E-2</v>
-      </c>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+        <f>D98*(C102*VLOOKUP(B102, 'Match Predictions'!$D$808:$Y$838, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$808:$Y$838, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$808:$Y$838, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$808:$Y$838, 21, FALSE))</f>
+        <v>3.9789613203299878E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>119</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>10</v>
+      <c r="B99" t="s">
+        <v>40</v>
       </c>
       <c r="C99" s="2">
-        <v>0.49780000000000002</v>
+        <v>0.34470000000000001</v>
       </c>
       <c r="D99" s="2">
-        <f t="shared" si="43"/>
-        <v>0.26479999999999992</v>
+        <v>0.38759999999999994</v>
       </c>
       <c r="E99" s="2">
-        <v>0.76259999999999994</v>
+        <v>0.73229999999999995</v>
       </c>
       <c r="F99" s="2">
-        <f>D99*(C102*VLOOKUP(B102, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$95:$Y$125, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$95:$Y$125, 21, FALSE))</f>
-        <v>0.11514190333256598</v>
-      </c>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B100" s="2"/>
+        <f>D99*(C102*VLOOKUP(B102, 'Match Predictions'!$D$839:$Y$869, 21, FALSE) + C103*VLOOKUP(B103, 'Match Predictions'!$D$839:$Y$869, 21, FALSE) + C104*VLOOKUP(B104, 'Match Predictions'!$D$839:$Y$869, 21, FALSE) + C105*VLOOKUP(B105, 'Match Predictions'!$D$839:$Y$869, 21, FALSE))</f>
+        <v>0.20793477124128112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C100" s="2">
-        <f t="shared" ref="C100" si="44">SUM(C96:C99)</f>
+        <f t="shared" ref="C100" si="42">SUM(C96:C99)</f>
         <v>1</v>
       </c>
       <c r="D100" s="2">
-        <f t="shared" ref="D100" si="45">SUM(D96:D99)</f>
+        <f t="shared" ref="D100" si="43">SUM(D96:D99)</f>
         <v>1</v>
       </c>
       <c r="E100" s="2">
-        <f t="shared" ref="E100" si="46">SUM(E96:E99)</f>
+        <f t="shared" ref="E100" si="44">SUM(E96:E99)</f>
         <v>2</v>
       </c>
       <c r="F100" s="2">
         <f>SUM(F96:F99)</f>
-        <v>0.30670824917806866</v>
-      </c>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B101" s="4" t="s">
+        <v>0.45839140387517013</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
         <v>85</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>120</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>11</v>
+      <c r="B102" t="s">
+        <v>41</v>
       </c>
       <c r="C102" s="2">
-        <v>0.24510000000000001</v>
+        <v>0.31690000000000002</v>
       </c>
       <c r="D102" s="2">
-        <f>E102-C102</f>
-        <v>0.27490000000000003</v>
+        <v>0.30229999999999996</v>
       </c>
       <c r="E102" s="2">
-        <v>0.52</v>
+        <v>0.61919999999999997</v>
       </c>
       <c r="F102" s="2">
-        <f>C102*(D96*VLOOKUP(B96, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$126:$Y$156, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$126:$Y$156, 21, FALSE))</f>
-        <v>0.16468071187978453</v>
-      </c>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+        <f>C102*(D96*VLOOKUP(B96, 'Match Predictions'!$D$870:$Y$900, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$870:$Y$900, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$870:$Y$900, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$870:$Y$900, 21, FALSE))</f>
+        <v>0.16703898235439635</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>121</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>13</v>
+      <c r="B103" t="s">
+        <v>43</v>
       </c>
       <c r="C103" s="2">
-        <v>0.44869999999999999</v>
+        <v>0.128</v>
       </c>
       <c r="D103" s="2">
-        <f>E103-C103</f>
-        <v>0.26890000000000003</v>
+        <v>0.22560000000000002</v>
       </c>
       <c r="E103" s="2">
-        <v>0.71760000000000002</v>
+        <v>0.35360000000000003</v>
       </c>
       <c r="F103" s="2">
-        <f>C103*(D96*VLOOKUP(B96, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$157:$Y$187, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$157:$Y$187, 21, FALSE))</f>
-        <v>0.34628468159497033</v>
-      </c>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+        <f>C103*(D96*VLOOKUP(B96, 'Match Predictions'!$D$901:$Y$931, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$901:$Y$931, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$901:$Y$931, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$901:$Y$931, 21, FALSE))</f>
+        <v>5.1368597959787848E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>122</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>14</v>
+      <c r="B104" t="s">
+        <v>44</v>
       </c>
       <c r="C104" s="2">
-        <v>0.19</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="D104" s="2">
-        <f>E104-C104</f>
-        <v>0.2555</v>
+        <v>0.28589999999999993</v>
       </c>
       <c r="E104" s="2">
-        <v>0.44550000000000001</v>
+        <v>0.74039999999999995</v>
       </c>
       <c r="F104" s="2">
-        <f>C104*(D96*VLOOKUP(B96, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$188:$Y$218, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$188:$Y$218, 21, FALSE))</f>
-        <v>0.11971051370413367</v>
-      </c>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+        <f>C104*(D96*VLOOKUP(B96, 'Match Predictions'!$D$932:$Y$962, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$932:$Y$962, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$932:$Y$962, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$932:$Y$962, 21, FALSE))</f>
+        <v>0.28626026382181519</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>123</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>15</v>
+      <c r="B105" t="s">
+        <v>45</v>
       </c>
       <c r="C105" s="2">
-        <v>0.1162</v>
+        <v>0.10059999999999999</v>
       </c>
       <c r="D105" s="2">
-        <f>E105-C105</f>
-        <v>0.20070000000000002</v>
+        <v>0.1862</v>
       </c>
       <c r="E105" s="2">
-        <v>0.31690000000000002</v>
+        <v>0.2868</v>
       </c>
       <c r="F105" s="2">
-        <f>C105*(D96*VLOOKUP(B96, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$219:$Y$249, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$219:$Y$249, 21, FALSE))</f>
-        <v>6.2615843643042735E-2</v>
-      </c>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B106" s="2"/>
+        <f>C105*(D96*VLOOKUP(B96, 'Match Predictions'!$D$963:$Y$993, 21, FALSE) + D97*VLOOKUP(B97, 'Match Predictions'!$D$963:$Y$993, 21, FALSE) + D98*VLOOKUP(B98, 'Match Predictions'!$D$963:$Y$993, 21, FALSE) + D99*VLOOKUP(B99, 'Match Predictions'!$D$963:$Y$993, 21, FALSE))</f>
+        <v>3.6940751988830532E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C106" s="2">
-        <f t="shared" ref="C106" si="47">SUM(C102:C105)</f>
-        <v>0.99999999999999989</v>
+        <f t="shared" ref="C106" si="45">SUM(C102:C105)</f>
+        <v>1</v>
       </c>
       <c r="D106" s="2">
-        <f t="shared" ref="D106" si="48">SUM(D102:D105)</f>
-        <v>1.0000000000000002</v>
+        <f t="shared" ref="D106" si="46">SUM(D102:D105)</f>
+        <v>1</v>
       </c>
       <c r="E106" s="2">
-        <f t="shared" ref="E106" si="49">SUM(E102:E105)</f>
+        <f t="shared" ref="E106" si="47">SUM(E102:E105)</f>
         <v>2</v>
       </c>
       <c r="F106" s="2">
         <f>SUM(F102:F105)</f>
-        <v>0.69329175082193129</v>
-      </c>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B107" s="2"/>
+        <v>0.54160859612482992</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -82366,23 +82050,6 @@
         <f>F106+F100</f>
         <v>1</v>
       </c>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F110" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>